<commit_message>
feat: implementando extração de valores da planilha
</commit_message>
<xml_diff>
--- a/sheets-processor-api/src/main/resources/planilha_clientes.xlsx
+++ b/sheets-processor-api/src/main/resources/planilha_clientes.xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A374181-53BA-4FE2-8E6A-253825DD43EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Responsável</t>
   </si>
@@ -40,58 +60,58 @@
     <t>Ana Silva</t>
   </si>
   <si>
+    <t>João Pereira</t>
+  </si>
+  <si>
+    <t>123.456.789-10</t>
+  </si>
+  <si>
+    <t>01000-000, Rua A, 123, Centro, São Paulo, SP</t>
+  </si>
+  <si>
+    <t>1990-01-01</t>
+  </si>
+  <si>
+    <t>joao.pereira@email.com</t>
+  </si>
+  <si>
+    <t>(11) 99999-9999</t>
+  </si>
+  <si>
     <t>Carlos Lima</t>
   </si>
   <si>
+    <t>Empresa XYZ</t>
+  </si>
+  <si>
+    <t>12.345.678/0001-99</t>
+  </si>
+  <si>
+    <t>02000-000, Av. B, 456, Jardim, Rio de Janeiro, RJ</t>
+  </si>
+  <si>
+    <t>contato@xyz.com</t>
+  </si>
+  <si>
+    <t>(21) 88888-8888</t>
+  </si>
+  <si>
     <t>Mariana Souza</t>
   </si>
   <si>
-    <t>João Pereira</t>
-  </si>
-  <si>
-    <t>Empresa XYZ</t>
-  </si>
-  <si>
     <t>Bruno Martins</t>
   </si>
   <si>
-    <t>123.456.789-10</t>
-  </si>
-  <si>
-    <t>12.345.678/0001-99</t>
-  </si>
-  <si>
     <t>987.654.321-00</t>
   </si>
   <si>
-    <t>01000-000, Rua A, 123, Centro, São Paulo, SP</t>
-  </si>
-  <si>
-    <t>02000-000, Av. B, 456, Jardim, Rio de Janeiro, RJ</t>
-  </si>
-  <si>
     <t>03000-000, Rua C, 789, Industrial, Belo Horizonte, MG</t>
   </si>
   <si>
-    <t>1990-01-01</t>
-  </si>
-  <si>
     <t>1985-05-10</t>
   </si>
   <si>
-    <t>joao.pereira@email.com</t>
-  </si>
-  <si>
-    <t>contato@xyz.com</t>
-  </si>
-  <si>
     <t>bruno.martins@email.com</t>
-  </si>
-  <si>
-    <t>(11) 99999-9999</t>
-  </si>
-  <si>
-    <t>(21) 88888-8888</t>
   </si>
   <si>
     <t>(31) 77777-7777</t>
@@ -100,14 +120,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -115,7 +135,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +183,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -172,10 +200,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -213,234 +241,128 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -451,12 +373,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.42578125" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -486,68 +419,76 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;KFF0000 CONFIDENTIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 CONFIDENTIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>